<commit_message>
export ficha proyecto api creado
</commit_message>
<xml_diff>
--- a/exports_app/templates/excel/proyecto_api.xlsx
+++ b/exports_app/templates/excel/proyecto_api.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basti\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basti\Escritorio\APIprojectBackend\exports_app\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60394E37-E8AE-4ABB-91EA-3ED4515C35C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E057D2A9-DF99-4208-A18C-D2D432903455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1647,7 +1647,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1689,9 +1689,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1722,17 +1719,326 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1748,315 +2054,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2087,7 +2084,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1800</xdr:colOff>
+      <xdr:colOff>1801</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>207424</xdr:rowOff>
     </xdr:to>
@@ -2434,20 +2431,21 @@
   </sheetPr>
   <dimension ref="B2:O64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A60" zoomScale="59" zoomScaleNormal="59" zoomScaleSheetLayoutView="59" workbookViewId="0">
-      <selection activeCell="M56" sqref="M56"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="59" zoomScaleNormal="59" zoomScaleSheetLayoutView="59" workbookViewId="0">
+      <selection activeCell="Q69" sqref="Q69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
-    <col min="8" max="10" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="32.42578125" customWidth="1"/>
+    <col min="8" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" customWidth="1"/>
     <col min="11" max="12" width="12.28515625" customWidth="1"/>
     <col min="13" max="13" width="22" customWidth="1"/>
     <col min="14" max="14" width="26.140625" customWidth="1"/>
@@ -2471,17 +2469,17 @@
       <c r="B5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
+      <c r="C6" s="103"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="103"/>
+      <c r="J6" s="103"/>
     </row>
     <row r="7" spans="2:10" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
@@ -2495,119 +2493,119 @@
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="136" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="36"/>
+      <c r="C8" s="137"/>
+      <c r="D8" s="138"/>
     </row>
     <row r="9" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="38"/>
+      <c r="C9" s="139"/>
+      <c r="D9" s="140"/>
     </row>
     <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="31"/>
+      <c r="C10" s="123"/>
+      <c r="D10" s="124"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="31"/>
+      <c r="C11" s="123"/>
+      <c r="D11" s="124"/>
     </row>
     <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="31"/>
+      <c r="C12" s="123"/>
+      <c r="D12" s="124"/>
     </row>
     <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="31"/>
+      <c r="C13" s="123"/>
+      <c r="D13" s="124"/>
     </row>
     <row r="14" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="45"/>
+      <c r="C14" s="125"/>
+      <c r="D14" s="126"/>
     </row>
     <row r="15" spans="2:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="C16" s="103"/>
+      <c r="D16" s="103"/>
+      <c r="E16" s="103"/>
+      <c r="F16" s="103"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="103"/>
+      <c r="I16" s="103"/>
+      <c r="J16" s="103"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="114" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="48"/>
+      <c r="C17" s="115"/>
+      <c r="D17" s="115"/>
+      <c r="E17" s="115"/>
+      <c r="F17" s="115"/>
+      <c r="G17" s="115"/>
+      <c r="H17" s="115"/>
+      <c r="I17" s="115"/>
+      <c r="J17" s="116"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="51"/>
+      <c r="C18" s="118"/>
+      <c r="D18" s="118"/>
+      <c r="E18" s="118"/>
+      <c r="F18" s="118"/>
+      <c r="G18" s="118"/>
+      <c r="H18" s="118"/>
+      <c r="I18" s="118"/>
+      <c r="J18" s="119"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="117" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="51"/>
+      <c r="C19" s="118"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="118"/>
+      <c r="F19" s="118"/>
+      <c r="G19" s="118"/>
+      <c r="H19" s="118"/>
+      <c r="I19" s="118"/>
+      <c r="J19" s="119"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="52" t="s">
+      <c r="B20" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="54"/>
+      <c r="C20" s="121"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="121"/>
+      <c r="F20" s="121"/>
+      <c r="G20" s="121"/>
+      <c r="H20" s="121"/>
+      <c r="I20" s="121"/>
+      <c r="J20" s="122"/>
     </row>
     <row r="22" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
@@ -2626,342 +2624,342 @@
       <c r="B23" s="7"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="55" t="s">
+      <c r="B24" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="56"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="58" t="s">
+      <c r="C24" s="128"/>
+      <c r="D24" s="129"/>
+      <c r="E24" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="59"/>
-      <c r="J24" s="60"/>
+      <c r="F24" s="131"/>
+      <c r="G24" s="131"/>
+      <c r="H24" s="131"/>
+      <c r="I24" s="131"/>
+      <c r="J24" s="132"/>
     </row>
     <row r="25" spans="2:10" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="62"/>
-      <c r="I25" s="62"/>
-      <c r="J25" s="63"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="133"/>
+      <c r="F25" s="134"/>
+      <c r="G25" s="134"/>
+      <c r="H25" s="134"/>
+      <c r="I25" s="134"/>
+      <c r="J25" s="135"/>
     </row>
     <row r="26" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="43"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="104"/>
+      <c r="F26" s="105"/>
+      <c r="G26" s="105"/>
+      <c r="H26" s="105"/>
+      <c r="I26" s="105"/>
+      <c r="J26" s="106"/>
     </row>
     <row r="27" spans="2:10" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="43"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="104"/>
+      <c r="F27" s="105"/>
+      <c r="G27" s="105"/>
+      <c r="H27" s="105"/>
+      <c r="I27" s="105"/>
+      <c r="J27" s="106"/>
     </row>
     <row r="28" spans="2:10" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="39" t="s">
+      <c r="B28" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="65"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="66"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="107"/>
+      <c r="F28" s="108"/>
+      <c r="G28" s="108"/>
+      <c r="H28" s="108"/>
+      <c r="I28" s="108"/>
+      <c r="J28" s="109"/>
     </row>
     <row r="29" spans="2:10" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="68"/>
-      <c r="G29" s="68"/>
-      <c r="H29" s="68"/>
-      <c r="I29" s="68"/>
-      <c r="J29" s="69"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="110"/>
+      <c r="F29" s="111"/>
+      <c r="G29" s="111"/>
+      <c r="H29" s="111"/>
+      <c r="I29" s="111"/>
+      <c r="J29" s="112"/>
     </row>
     <row r="31" spans="2:10" s="5" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="70" t="s">
+      <c r="B31" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="70"/>
-      <c r="D31" s="70"/>
-      <c r="E31" s="70"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="70"/>
-      <c r="H31" s="70"/>
-      <c r="I31" s="70"/>
-      <c r="J31" s="70"/>
+      <c r="C31" s="113"/>
+      <c r="D31" s="113"/>
+      <c r="E31" s="113"/>
+      <c r="F31" s="113"/>
+      <c r="G31" s="113"/>
+      <c r="H31" s="113"/>
+      <c r="I31" s="113"/>
+      <c r="J31" s="113"/>
     </row>
     <row r="32" spans="2:10" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
     </row>
     <row r="33" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
+      <c r="C33" s="103"/>
+      <c r="D33" s="103"/>
+      <c r="E33" s="103"/>
+      <c r="F33" s="103"/>
+      <c r="G33" s="103"/>
+      <c r="H33" s="103"/>
+      <c r="I33" s="103"/>
+      <c r="J33" s="103"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="46" t="s">
+      <c r="B34" s="114" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="47"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="48"/>
+      <c r="C34" s="115"/>
+      <c r="D34" s="115"/>
+      <c r="E34" s="115"/>
+      <c r="F34" s="115"/>
+      <c r="G34" s="115"/>
+      <c r="H34" s="115"/>
+      <c r="I34" s="115"/>
+      <c r="J34" s="116"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="50"/>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="51"/>
+      <c r="C35" s="118"/>
+      <c r="D35" s="118"/>
+      <c r="E35" s="118"/>
+      <c r="F35" s="118"/>
+      <c r="G35" s="118"/>
+      <c r="H35" s="118"/>
+      <c r="I35" s="118"/>
+      <c r="J35" s="119"/>
     </row>
     <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="52" t="s">
+      <c r="B36" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
-      <c r="G36" s="53"/>
-      <c r="H36" s="53"/>
-      <c r="I36" s="53"/>
-      <c r="J36" s="54"/>
+      <c r="C36" s="121"/>
+      <c r="D36" s="121"/>
+      <c r="E36" s="121"/>
+      <c r="F36" s="121"/>
+      <c r="G36" s="121"/>
+      <c r="H36" s="121"/>
+      <c r="I36" s="121"/>
+      <c r="J36" s="122"/>
     </row>
     <row r="38" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="32" t="s">
+      <c r="B38" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="33"/>
-      <c r="J38" s="33"/>
+      <c r="C38" s="103"/>
+      <c r="D38" s="103"/>
+      <c r="E38" s="103"/>
+      <c r="F38" s="103"/>
+      <c r="G38" s="103"/>
+      <c r="H38" s="103"/>
+      <c r="I38" s="103"/>
+      <c r="J38" s="103"/>
     </row>
     <row r="39" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="71" t="s">
+      <c r="B39" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="72"/>
-      <c r="D39" s="73"/>
-      <c r="E39" s="74" t="s">
+      <c r="C39" s="91"/>
+      <c r="D39" s="92"/>
+      <c r="E39" s="93" t="s">
         <v>30</v>
       </c>
-      <c r="F39" s="75"/>
-      <c r="G39" s="76"/>
-      <c r="H39" s="74" t="s">
+      <c r="F39" s="94"/>
+      <c r="G39" s="95"/>
+      <c r="H39" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="I39" s="75"/>
-      <c r="J39" s="76"/>
+      <c r="I39" s="94"/>
+      <c r="J39" s="95"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="77"/>
-      <c r="C40" s="78"/>
-      <c r="D40" s="79"/>
-      <c r="E40" s="80"/>
-      <c r="F40" s="81"/>
-      <c r="G40" s="82"/>
-      <c r="H40" s="83"/>
-      <c r="I40" s="81"/>
-      <c r="J40" s="82"/>
+      <c r="B40" s="96"/>
+      <c r="C40" s="97"/>
+      <c r="D40" s="98"/>
+      <c r="E40" s="99"/>
+      <c r="F40" s="100"/>
+      <c r="G40" s="101"/>
+      <c r="H40" s="102"/>
+      <c r="I40" s="100"/>
+      <c r="J40" s="101"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="84"/>
-      <c r="C41" s="85"/>
-      <c r="D41" s="86"/>
-      <c r="E41" s="87"/>
-      <c r="F41" s="88"/>
-      <c r="G41" s="89"/>
-      <c r="H41" s="90"/>
-      <c r="I41" s="88"/>
-      <c r="J41" s="89"/>
+      <c r="B41" s="83"/>
+      <c r="C41" s="84"/>
+      <c r="D41" s="85"/>
+      <c r="E41" s="86"/>
+      <c r="F41" s="87"/>
+      <c r="G41" s="88"/>
+      <c r="H41" s="89"/>
+      <c r="I41" s="87"/>
+      <c r="J41" s="88"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="84"/>
-      <c r="C42" s="85"/>
-      <c r="D42" s="86"/>
-      <c r="E42" s="87"/>
-      <c r="F42" s="88"/>
-      <c r="G42" s="89"/>
-      <c r="H42" s="90"/>
-      <c r="I42" s="88"/>
-      <c r="J42" s="89"/>
+      <c r="B42" s="83"/>
+      <c r="C42" s="84"/>
+      <c r="D42" s="85"/>
+      <c r="E42" s="86"/>
+      <c r="F42" s="87"/>
+      <c r="G42" s="88"/>
+      <c r="H42" s="89"/>
+      <c r="I42" s="87"/>
+      <c r="J42" s="88"/>
     </row>
     <row r="43" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="91"/>
-      <c r="C43" s="92"/>
-      <c r="D43" s="93"/>
-      <c r="E43" s="94"/>
-      <c r="F43" s="95"/>
-      <c r="G43" s="96"/>
-      <c r="H43" s="97"/>
-      <c r="I43" s="95"/>
-      <c r="J43" s="96"/>
+      <c r="B43" s="68"/>
+      <c r="C43" s="69"/>
+      <c r="D43" s="70"/>
+      <c r="E43" s="71"/>
+      <c r="F43" s="72"/>
+      <c r="G43" s="73"/>
+      <c r="H43" s="74"/>
+      <c r="I43" s="72"/>
+      <c r="J43" s="73"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="8"/>
     </row>
     <row r="45" spans="2:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="32" t="s">
+      <c r="B45" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="32"/>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="46"/>
+      <c r="I45" s="46"/>
+      <c r="J45" s="46"/>
     </row>
     <row r="46" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="98" t="s">
+      <c r="B47" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="99"/>
-      <c r="D47" s="100"/>
-      <c r="E47" s="101" t="s">
+      <c r="C47" s="76"/>
+      <c r="D47" s="77"/>
+      <c r="E47" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="F47" s="102"/>
-      <c r="G47" s="103"/>
-      <c r="I47" s="104" t="s">
+      <c r="F47" s="79"/>
+      <c r="G47" s="80"/>
+      <c r="I47" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="J47" s="105"/>
-    </row>
-    <row r="48" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="39" t="s">
+      <c r="J47" s="82"/>
+    </row>
+    <row r="48" spans="2:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="C48" s="40"/>
-      <c r="D48" s="106"/>
-      <c r="E48" s="107"/>
-      <c r="F48" s="108"/>
-      <c r="G48" s="109"/>
-      <c r="H48" s="110" t="s">
+      <c r="C48" s="49"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="52"/>
+      <c r="G48" s="53"/>
+      <c r="H48" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="I48" s="111"/>
-      <c r="J48" s="112"/>
-    </row>
-    <row r="49" spans="2:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="39" t="s">
+      <c r="I48" s="55"/>
+      <c r="J48" s="56"/>
+    </row>
+    <row r="49" spans="2:15" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="C49" s="40"/>
-      <c r="D49" s="106"/>
-      <c r="E49" s="117"/>
-      <c r="F49" s="118"/>
-      <c r="G49" s="119"/>
-      <c r="H49" s="110"/>
-      <c r="I49" s="113"/>
-      <c r="J49" s="114"/>
-    </row>
-    <row r="50" spans="2:15" ht="60.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="39" t="s">
+      <c r="C49" s="49"/>
+      <c r="D49" s="50"/>
+      <c r="E49" s="61"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="62"/>
+      <c r="H49" s="54"/>
+      <c r="I49" s="57"/>
+      <c r="J49" s="58"/>
+    </row>
+    <row r="50" spans="2:15" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="C50" s="40"/>
-      <c r="D50" s="106"/>
-      <c r="E50" s="117"/>
-      <c r="F50" s="118"/>
-      <c r="G50" s="119"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="61"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="62"/>
       <c r="H50" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="I50" s="113"/>
-      <c r="J50" s="114"/>
-    </row>
-    <row r="51" spans="2:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="39" t="s">
+      <c r="I50" s="57"/>
+      <c r="J50" s="58"/>
+    </row>
+    <row r="51" spans="2:15" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="C51" s="40"/>
-      <c r="D51" s="106"/>
-      <c r="E51" s="117"/>
-      <c r="F51" s="118"/>
-      <c r="G51" s="119"/>
-      <c r="I51" s="113"/>
-      <c r="J51" s="114"/>
-    </row>
-    <row r="52" spans="2:15" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="120" t="s">
+      <c r="C51" s="49"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="61"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="62"/>
+      <c r="I51" s="57"/>
+      <c r="J51" s="58"/>
+    </row>
+    <row r="52" spans="2:15" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="C52" s="121"/>
-      <c r="D52" s="122"/>
-      <c r="E52" s="123"/>
-      <c r="F52" s="124"/>
-      <c r="G52" s="125"/>
-      <c r="I52" s="115"/>
-      <c r="J52" s="116"/>
+      <c r="C52" s="64"/>
+      <c r="D52" s="65"/>
+      <c r="E52" s="66"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="67"/>
+      <c r="I52" s="59"/>
+      <c r="J52" s="60"/>
     </row>
     <row r="53" spans="2:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="11"/>
     </row>
     <row r="54" spans="2:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="126" t="s">
+      <c r="B54" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C54" s="126"/>
-      <c r="D54" s="126"/>
-      <c r="E54" s="126"/>
-      <c r="F54" s="126"/>
-      <c r="G54" s="126"/>
-      <c r="H54" s="126"/>
-      <c r="I54" s="126"/>
-      <c r="J54" s="126"/>
+      <c r="C54" s="45"/>
+      <c r="D54" s="45"/>
+      <c r="E54" s="45"/>
+      <c r="F54" s="45"/>
+      <c r="G54" s="45"/>
+      <c r="H54" s="45"/>
+      <c r="I54" s="45"/>
+      <c r="J54" s="45"/>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" s="12"/>
@@ -2971,17 +2969,17 @@
       <c r="F55" s="13"/>
     </row>
     <row r="56" spans="2:15" ht="168" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="32" t="s">
+      <c r="B56" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="C56" s="32"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="32"/>
-      <c r="H56" s="32"/>
-      <c r="I56" s="32"/>
-      <c r="J56" s="32"/>
+      <c r="C56" s="46"/>
+      <c r="D56" s="46"/>
+      <c r="E56" s="46"/>
+      <c r="F56" s="46"/>
+      <c r="G56" s="46"/>
+      <c r="H56" s="46"/>
+      <c r="I56" s="46"/>
+      <c r="J56" s="46"/>
     </row>
     <row r="57" spans="2:15" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="11"/>
@@ -2990,29 +2988,29 @@
       <c r="B58" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C58" s="127" t="s">
+      <c r="C58" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="D58" s="128"/>
+      <c r="D58" s="40"/>
       <c r="E58" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="F58" s="128" t="s">
+      <c r="F58" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="G58" s="128"/>
-      <c r="H58" s="128" t="s">
+      <c r="G58" s="40"/>
+      <c r="H58" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="I58" s="128"/>
-      <c r="J58" s="128" t="s">
+      <c r="I58" s="40"/>
+      <c r="J58" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="K58" s="128"/>
-      <c r="L58" s="128" t="s">
+      <c r="K58" s="40"/>
+      <c r="L58" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="M58" s="129"/>
+      <c r="M58" s="41"/>
       <c r="N58" s="14" t="s">
         <v>51</v>
       </c>
@@ -3021,66 +3019,68 @@
       </c>
     </row>
     <row r="59" spans="2:15" ht="409.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="22"/>
-      <c r="C59" s="130"/>
-      <c r="D59" s="131"/>
-      <c r="E59" s="24"/>
-      <c r="F59" s="131"/>
-      <c r="G59" s="131"/>
-      <c r="H59" s="132"/>
-      <c r="I59" s="133"/>
-      <c r="J59" s="131"/>
-      <c r="K59" s="131"/>
-      <c r="L59" s="132"/>
-      <c r="M59" s="133"/>
-      <c r="N59" s="25"/>
-      <c r="O59" s="25"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="42"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="34"/>
+      <c r="G59" s="34"/>
+      <c r="H59" s="43"/>
+      <c r="I59" s="44"/>
+      <c r="J59" s="34"/>
+      <c r="K59" s="34"/>
+      <c r="L59" s="43"/>
+      <c r="M59" s="44"/>
+      <c r="N59" s="24"/>
+      <c r="O59" s="24"/>
     </row>
     <row r="60" spans="2:15" ht="409.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="26"/>
-      <c r="C60" s="141"/>
-      <c r="D60" s="118"/>
-      <c r="E60" s="28"/>
-      <c r="F60" s="131"/>
-      <c r="G60" s="131"/>
-      <c r="H60" s="118"/>
-      <c r="I60" s="118"/>
-      <c r="J60" s="131"/>
-      <c r="K60" s="131"/>
-      <c r="L60" s="124"/>
-      <c r="M60" s="124"/>
-      <c r="N60" s="23"/>
-      <c r="O60" s="23"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="33"/>
+      <c r="E60" s="27"/>
+      <c r="F60" s="34"/>
+      <c r="G60" s="34"/>
+      <c r="H60" s="33"/>
+      <c r="I60" s="33"/>
+      <c r="J60" s="34"/>
+      <c r="K60" s="34"/>
+      <c r="L60" s="35"/>
+      <c r="M60" s="35"/>
+      <c r="N60" s="22"/>
+      <c r="O60" s="22"/>
     </row>
     <row r="61" spans="2:15" ht="409.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="26"/>
-      <c r="C61" s="134"/>
-      <c r="D61" s="135"/>
-      <c r="E61" s="27"/>
-      <c r="F61" s="136"/>
-      <c r="G61" s="136"/>
-      <c r="H61" s="135"/>
-      <c r="I61" s="135"/>
-      <c r="J61" s="136"/>
-      <c r="K61" s="136"/>
-      <c r="L61" s="137"/>
-      <c r="M61" s="137"/>
-      <c r="N61" s="29"/>
-      <c r="O61" s="29"/>
-    </row>
-    <row r="62" spans="2:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="16"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
-      <c r="K62" s="4"/>
-      <c r="L62" s="4"/>
-      <c r="M62" s="4"/>
+      <c r="B61" s="25"/>
+      <c r="C61" s="36"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="38"/>
+      <c r="H61" s="37"/>
+      <c r="I61" s="37"/>
+      <c r="J61" s="38"/>
+      <c r="K61" s="38"/>
+      <c r="L61" s="39"/>
+      <c r="M61" s="39"/>
+      <c r="N61" s="28"/>
+      <c r="O61" s="28"/>
+    </row>
+    <row r="62" spans="2:15" ht="337.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="25"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="37"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="38"/>
+      <c r="G62" s="38"/>
+      <c r="H62" s="37"/>
+      <c r="I62" s="37"/>
+      <c r="J62" s="38"/>
+      <c r="K62" s="38"/>
+      <c r="L62" s="39"/>
+      <c r="M62" s="39"/>
+      <c r="N62" s="28"/>
+      <c r="O62" s="28"/>
     </row>
     <row r="63" spans="2:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B63" s="6" t="s">
@@ -3095,86 +3095,27 @@
       <c r="M63" s="4"/>
     </row>
     <row r="64" spans="2:15" ht="159" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="138" t="s">
+      <c r="B64" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C64" s="139"/>
-      <c r="D64" s="139"/>
-      <c r="E64" s="139"/>
-      <c r="F64" s="139"/>
-      <c r="G64" s="139"/>
-      <c r="H64" s="139"/>
-      <c r="I64" s="139"/>
-      <c r="J64" s="140"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="30"/>
+      <c r="G64" s="30"/>
+      <c r="H64" s="30"/>
+      <c r="I64" s="30"/>
+      <c r="J64" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="85">
-    <mergeCell ref="B64:J64"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="J60:K60"/>
-    <mergeCell ref="L60:M60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="J61:K61"/>
-    <mergeCell ref="L61:M61"/>
-    <mergeCell ref="L58:M58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="J59:K59"/>
-    <mergeCell ref="L59:M59"/>
-    <mergeCell ref="B54:J54"/>
-    <mergeCell ref="B56:J56"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="H48:H49"/>
-    <mergeCell ref="I48:J52"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="B45:J45"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:J41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="B38:J38"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="B31:J31"/>
-    <mergeCell ref="B33:J33"/>
-    <mergeCell ref="B34:J34"/>
-    <mergeCell ref="B35:J35"/>
-    <mergeCell ref="B36:J36"/>
+  <mergeCells count="90">
+    <mergeCell ref="L62:M62"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="E26:J26"/>
     <mergeCell ref="C13:D13"/>
@@ -3188,12 +3129,76 @@
     <mergeCell ref="E24:J24"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="E25:J25"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="B38:J38"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="B31:J31"/>
+    <mergeCell ref="B33:J33"/>
+    <mergeCell ref="B34:J34"/>
+    <mergeCell ref="B35:J35"/>
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:J41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="B45:J45"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="H48:H49"/>
+    <mergeCell ref="I48:J52"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="B54:J54"/>
+    <mergeCell ref="B56:J56"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="L58:M58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="J59:K59"/>
+    <mergeCell ref="L59:M59"/>
+    <mergeCell ref="L60:M60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="J61:K61"/>
+    <mergeCell ref="L61:M61"/>
+    <mergeCell ref="B64:J64"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="J60:K60"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="J62:K62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="44" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -3205,6 +3210,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="4c7ad61e-cff9-489a-be31-94530e6ea8e8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FE379DBB0AEC2844B6FDAE608D32181C" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3a4e7d32c19bd719b46d88525627461c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="07ca096b-2cdc-4848-8c4e-6a9cb17e0f3c" xmlns:ns4="4c7ad61e-cff9-489a-be31-94530e6ea8e8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="45b185b727612748de2216de031ff1ac" ns3:_="" ns4:_="">
     <xsd:import namespace="07ca096b-2cdc-4848-8c4e-6a9cb17e0f3c"/>
@@ -3437,24 +3459,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="4c7ad61e-cff9-489a-be31-94530e6ea8e8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AA9A2C-EA00-415A-9D13-6C8EFB6423D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89B774FC-7725-43CC-B68A-3A6642FB3BAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4c7ad61e-cff9-489a-be31-94530e6ea8e8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13171D30-8DCB-4439-94FA-73216F0AFCCB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3471,22 +3494,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89B774FC-7725-43CC-B68A-3A6642FB3BAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4c7ad61e-cff9-489a-be31-94530e6ea8e8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AA9A2C-EA00-415A-9D13-6C8EFB6423D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>